<commit_message>
add sitcp test code
</commit_message>
<xml_diff>
--- a/template/u4FCPv1/KUP/sitcp-fmc1_dp0/sources/wishbone/wb_reg/reg_table.xlsx
+++ b/template/u4FCPv1/KUP/sitcp-fmc1_dp0/sources/wishbone/wb_reg/reg_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
   <si>
     <t xml:space="preserve">block name</t>
   </si>
@@ -98,6 +98,108 @@
   </si>
   <si>
     <t xml:space="preserve">Firmware Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fpga_dna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FPGA DNA ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp_mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCP mode: 2’b01 - Loopback mode, 2’b10 - Test mode, 2’b00 – Normal mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp_test_tx_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default: 0x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmission data rate in units of 100 Mbps for TCP test mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp_test_num_of_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default: 0x4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of bytes to be transmitted for TCP test mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp_test_data_gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data transmission enable for TCP test mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp_test_word_len</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default: 0x7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Word length of test data for one clock cycle for TCP test mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp_test_select_seq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use the sequence pattern as defined below for TCP test mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp_test_seq_pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default: 0x60808040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequence pattern, each 4-bit define the number of bytes for one clock cycle  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp_test_blk_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default: 0x400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmission block size in bytes for TCP test mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcp_test_ins_error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w1trg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data error insertion for TCP test mode</t>
   </si>
 </sst>
 </file>
@@ -181,7 +283,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -203,6 +305,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,13 +336,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.63"/>
@@ -415,7 +521,177 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="0"/>
+      <c r="G10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="0"/>
+      <c r="G13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="0"/>
+      <c r="G17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="0"/>
+      <c r="G18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>